<commit_message>
Update BASE - VENDA E REGISTRO.xlsx
</commit_message>
<xml_diff>
--- a/BASE - VENDA E REGISTRO.xlsx
+++ b/BASE - VENDA E REGISTRO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Viana e Moura\Dropbox\PLANEJAMENTO\Scripts\MÓDULO VENDAS\MODULO_VENDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61859730-EC81-4A23-B6B1-184B3A585DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FDEDF2-8EF7-44F8-A25D-D3A1C54C5340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0382C43D-564D-4A4C-8EAB-6952E70C6A7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0382C43D-564D-4A4C-8EAB-6952E70C6A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="PLANEJADOR MÓDULOS" sheetId="1" r:id="rId1"/>
@@ -175,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="72">
   <si>
     <t>PROGRAMAÇÃO
  DOCUMENTAÇÕES</t>
@@ -389,6 +389,9 @@
   </si>
   <si>
     <t>SÃO VICENTE III-MERID(E)-09</t>
+  </si>
+  <si>
+    <t>"-"</t>
   </si>
 </sst>
 </file>
@@ -757,6 +760,9 @@
     <xf numFmtId="14" fontId="12" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -767,9 +773,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1189,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95DB70CC-ACBF-416D-B448-0645472647BA}">
   <dimension ref="A2:AN27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AG27" sqref="AG27"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AJ20" sqref="AJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="10.8" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1261,54 +1264,54 @@
     </row>
     <row r="3" spans="1:40" ht="10.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="41" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="K3" s="38" t="s">
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="K3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="P3" s="41" t="s">
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="P3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="U3" s="38" t="s">
+      <c r="Q3" s="42"/>
+      <c r="R3" s="42"/>
+      <c r="S3" s="42"/>
+      <c r="U3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="V3" s="38"/>
-      <c r="W3" s="38"/>
-      <c r="X3" s="38"/>
-      <c r="Z3" s="38" t="s">
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Z3" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="AA3" s="38"/>
-      <c r="AB3" s="38"/>
-      <c r="AC3" s="38"/>
-      <c r="AE3" s="38" t="s">
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AE3" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="AF3" s="38"/>
-      <c r="AG3" s="38"/>
-      <c r="AH3" s="39"/>
-      <c r="AJ3" s="38" t="s">
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="40"/>
+      <c r="AJ3" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="AK3" s="38"/>
-      <c r="AL3" s="38"/>
-      <c r="AM3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="39"/>
+      <c r="AM3" s="40"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
@@ -2855,8 +2858,8 @@
       <c r="AE17" s="23">
         <v>46054</v>
       </c>
-      <c r="AF17" s="37">
-        <v>46079</v>
+      <c r="AF17" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="AG17" s="28">
         <f t="shared" si="7"/>
@@ -2867,13 +2870,13 @@
         <v>151</v>
       </c>
       <c r="AI17" s="22"/>
-      <c r="AJ17" s="23">
+      <c r="AJ17" s="23" t="str">
         <f t="shared" si="20"/>
-        <v>46080</v>
-      </c>
-      <c r="AK17" s="19">
+        <v>-</v>
+      </c>
+      <c r="AK17" s="19" t="str">
         <f t="shared" si="21"/>
-        <v>46100</v>
+        <v>-</v>
       </c>
       <c r="AL17" s="28">
         <f t="shared" si="22"/>
@@ -2883,9 +2886,9 @@
         <f t="shared" si="23"/>
         <v>172</v>
       </c>
-      <c r="AN17" s="17">
+      <c r="AN17" s="17" t="str">
         <f t="shared" si="8"/>
-        <v>-45928</v>
+        <v>-</v>
       </c>
     </row>
     <row r="18" spans="2:40" x14ac:dyDescent="0.25">
@@ -2977,8 +2980,8 @@
       <c r="AE18" s="23">
         <v>46023</v>
       </c>
-      <c r="AF18" s="37">
-        <v>46050</v>
+      <c r="AF18" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="AG18" s="28">
         <f t="shared" si="7"/>
@@ -2989,13 +2992,13 @@
         <v>151</v>
       </c>
       <c r="AI18" s="22"/>
-      <c r="AJ18" s="23">
+      <c r="AJ18" s="23" t="str">
         <f t="shared" si="20"/>
-        <v>46051</v>
-      </c>
-      <c r="AK18" s="19">
+        <v>-</v>
+      </c>
+      <c r="AK18" s="19" t="str">
         <f t="shared" si="21"/>
-        <v>46071</v>
+        <v>-</v>
       </c>
       <c r="AL18" s="28">
         <f t="shared" si="22"/>
@@ -3005,9 +3008,9 @@
         <f t="shared" si="23"/>
         <v>172</v>
       </c>
-      <c r="AN18" s="17">
+      <c r="AN18" s="17" t="str">
         <f t="shared" si="8"/>
-        <v>-45899</v>
+        <v>-</v>
       </c>
     </row>
     <row r="19" spans="2:40" x14ac:dyDescent="0.25">
@@ -3099,8 +3102,8 @@
       <c r="AE19" s="23">
         <v>46082</v>
       </c>
-      <c r="AF19" s="37">
-        <v>46107</v>
+      <c r="AF19" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="AG19" s="28">
         <f t="shared" si="7"/>
@@ -3111,13 +3114,13 @@
         <v>151</v>
       </c>
       <c r="AI19" s="22"/>
-      <c r="AJ19" s="23">
+      <c r="AJ19" s="23" t="str">
         <f t="shared" si="20"/>
-        <v>46108</v>
-      </c>
-      <c r="AK19" s="19">
+        <v>-</v>
+      </c>
+      <c r="AK19" s="19" t="str">
         <f t="shared" si="21"/>
-        <v>46128</v>
+        <v>-</v>
       </c>
       <c r="AL19" s="28">
         <f t="shared" si="22"/>
@@ -3127,9 +3130,9 @@
         <f t="shared" si="23"/>
         <v>172</v>
       </c>
-      <c r="AN19" s="17">
+      <c r="AN19" s="17" t="str">
         <f t="shared" si="8"/>
-        <v>-45956</v>
+        <v>-</v>
       </c>
     </row>
     <row r="20" spans="2:40" x14ac:dyDescent="0.25">
@@ -3221,8 +3224,8 @@
       <c r="AE20" s="23">
         <v>46113</v>
       </c>
-      <c r="AF20" s="37">
-        <v>46140</v>
+      <c r="AF20" s="37" t="s">
+        <v>71</v>
       </c>
       <c r="AG20" s="28">
         <f t="shared" si="7"/>
@@ -3233,13 +3236,13 @@
         <v>151</v>
       </c>
       <c r="AI20" s="22"/>
-      <c r="AJ20" s="23">
+      <c r="AJ20" s="23" t="str">
         <f t="shared" si="20"/>
-        <v>46141</v>
-      </c>
-      <c r="AK20" s="19">
+        <v>-</v>
+      </c>
+      <c r="AK20" s="19" t="str">
         <f t="shared" si="21"/>
-        <v>46161</v>
+        <v>-</v>
       </c>
       <c r="AL20" s="28">
         <f t="shared" si="22"/>
@@ -3249,13 +3252,13 @@
         <f t="shared" si="23"/>
         <v>172</v>
       </c>
-      <c r="AN20" s="17">
+      <c r="AN20" s="17" t="str">
         <f t="shared" si="8"/>
-        <v>-45989</v>
+        <v>-</v>
       </c>
     </row>
     <row r="27" spans="2:40" x14ac:dyDescent="0.25">
-      <c r="AG27" s="42"/>
+      <c r="AG27" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>